<commit_message>
Add task to run npm on start
</commit_message>
<xml_diff>
--- a/ml/resultados.xlsx
+++ b/ml/resultados.xlsx
@@ -476,16 +476,16 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>942.0330900243309</v>
+        <v>941.648499594485</v>
       </c>
       <c r="C2" t="n">
-        <v>13.95496856688823</v>
+        <v>14.33266132095963</v>
       </c>
       <c r="D2" t="n">
-        <v>947.6150774510862</v>
+        <v>947.3815641228688</v>
       </c>
       <c r="E2" t="n">
-        <v>936.4511025975756</v>
+        <v>935.9154350661012</v>
       </c>
     </row>
     <row r="3">
@@ -495,16 +495,16 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1029.057797611961</v>
+        <v>1029.171806258189</v>
       </c>
       <c r="C3" t="n">
-        <v>6.393864010264351</v>
+        <v>6.542196503806269</v>
       </c>
       <c r="D3" t="n">
-        <v>1031.615343216067</v>
+        <v>1031.788684859712</v>
       </c>
       <c r="E3" t="n">
-        <v>1026.500252007855</v>
+        <v>1026.554927656667</v>
       </c>
     </row>
     <row r="4">
@@ -514,16 +514,16 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1039.608272506083</v>
+        <v>1037.977615571776</v>
       </c>
       <c r="C4" t="n">
-        <v>4.93175621133443</v>
+        <v>4.994760902097197</v>
       </c>
       <c r="D4" t="n">
-        <v>1041.580974990617</v>
+        <v>1039.975519932615</v>
       </c>
       <c r="E4" t="n">
-        <v>1037.635570021549</v>
+        <v>1035.979711210937</v>
       </c>
     </row>
     <row r="5">
@@ -533,16 +533,16 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1041.447378094304</v>
+        <v>1044.741419945683</v>
       </c>
       <c r="C5" t="n">
-        <v>10.21824216507905</v>
+        <v>11.96320906192886</v>
       </c>
       <c r="D5" t="n">
-        <v>1045.534674960336</v>
+        <v>1049.526703570455</v>
       </c>
       <c r="E5" t="n">
-        <v>1037.360081228272</v>
+        <v>1039.956136320911</v>
       </c>
     </row>
     <row r="6">
@@ -552,16 +552,16 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1057.875501868811</v>
+        <v>1057.48675713591</v>
       </c>
       <c r="C6" t="n">
-        <v>6.321680621758998</v>
+        <v>5.569991493540691</v>
       </c>
       <c r="D6" t="n">
-        <v>1060.404174117515</v>
+        <v>1059.714753733326</v>
       </c>
       <c r="E6" t="n">
-        <v>1055.346829620108</v>
+        <v>1055.258760538494</v>
       </c>
     </row>
     <row r="7">
@@ -571,16 +571,16 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1158.831132978825</v>
+        <v>1153.195801172311</v>
       </c>
       <c r="C7" t="n">
-        <v>24.99600378781001</v>
+        <v>26.23851309646741</v>
       </c>
       <c r="D7" t="n">
-        <v>1168.829534493949</v>
+        <v>1163.691206410898</v>
       </c>
       <c r="E7" t="n">
-        <v>1148.832731463701</v>
+        <v>1142.700395933724</v>
       </c>
     </row>
     <row r="8">
@@ -590,54 +590,54 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1167.939834046592</v>
+        <v>1160.502460495646</v>
       </c>
       <c r="C8" t="n">
-        <v>26.25699383175943</v>
+        <v>25.04180926258941</v>
       </c>
       <c r="D8" t="n">
-        <v>1178.442631579296</v>
+        <v>1170.519184200681</v>
       </c>
       <c r="E8" t="n">
-        <v>1157.437036513888</v>
+        <v>1150.48573679061</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>RandomForestClassifier</t>
+          <t xml:space="preserve"> DecisionTreeClassifier</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>1322.713381995134</v>
+        <v>1313.860178426602</v>
       </c>
       <c r="C9" t="n">
-        <v>31.92158948938673</v>
+        <v>43.70057545353648</v>
       </c>
       <c r="D9" t="n">
-        <v>1335.482017790889</v>
+        <v>1331.340408608016</v>
       </c>
       <c r="E9" t="n">
-        <v>1309.944746199379</v>
+        <v>1296.379948245187</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t xml:space="preserve"> DecisionTreeClassifier</t>
+          <t>RandomForestClassifier</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>1335.171938361719</v>
+        <v>1326.859529602595</v>
       </c>
       <c r="C10" t="n">
-        <v>44.53719848316565</v>
+        <v>36.87193292599426</v>
       </c>
       <c r="D10" t="n">
-        <v>1352.986817754986</v>
+        <v>1341.608302772993</v>
       </c>
       <c r="E10" t="n">
-        <v>1317.357058968453</v>
+        <v>1312.110756432198</v>
       </c>
     </row>
     <row r="11">
@@ -647,16 +647,16 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>1359.765369018654</v>
+        <v>1360.565477155988</v>
       </c>
       <c r="C11" t="n">
-        <v>37.10852217484386</v>
+        <v>18.67480558986908</v>
       </c>
       <c r="D11" t="n">
-        <v>1374.608777888591</v>
+        <v>1368.035399391936</v>
       </c>
       <c r="E11" t="n">
-        <v>1344.921960148716</v>
+        <v>1353.095554920041</v>
       </c>
     </row>
     <row r="12">
@@ -666,16 +666,16 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>1420.547120843471</v>
+        <v>1444.570478507705</v>
       </c>
       <c r="C12" t="n">
-        <v>49.07448766427523</v>
+        <v>83.42927554568691</v>
       </c>
       <c r="D12" t="n">
-        <v>1440.176915909181</v>
+        <v>1477.94218872598</v>
       </c>
       <c r="E12" t="n">
-        <v>1400.917325777761</v>
+        <v>1411.19876828943</v>
       </c>
     </row>
   </sheetData>
@@ -986,16 +986,16 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>938.4373073803731</v>
+        <v>938.597891321979</v>
       </c>
       <c r="C2" t="n">
-        <v>15.58573318062979</v>
+        <v>15.21431862768141</v>
       </c>
       <c r="D2" t="n">
-        <v>944.671600652625</v>
+        <v>944.6836187730515</v>
       </c>
       <c r="E2" t="n">
-        <v>932.2030141081212</v>
+        <v>932.5121638709064</v>
       </c>
     </row>
     <row r="3">
@@ -1005,54 +1005,54 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1028.555465673918</v>
+        <v>1028.671944487952</v>
       </c>
       <c r="C3" t="n">
-        <v>6.953552912760779</v>
+        <v>7.063978882572012</v>
       </c>
       <c r="D3" t="n">
-        <v>1031.336886839022</v>
+        <v>1031.497536040981</v>
       </c>
       <c r="E3" t="n">
-        <v>1025.774044508813</v>
+        <v>1025.846352934924</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>GradientBoostingRegressor</t>
+          <t>KNN</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1042.720589290487</v>
+        <v>1041.654176804542</v>
       </c>
       <c r="C4" t="n">
-        <v>16.77444729701994</v>
+        <v>4.02575937202237</v>
       </c>
       <c r="D4" t="n">
-        <v>1049.430368209295</v>
+        <v>1043.264480553351</v>
       </c>
       <c r="E4" t="n">
-        <v>1036.010810371679</v>
+        <v>1040.043873055733</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>KNN</t>
+          <t>GradientBoostingRegressor</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1043.409570154096</v>
+        <v>1041.760408373591</v>
       </c>
       <c r="C5" t="n">
-        <v>3.213827087159832</v>
+        <v>18.49235219597699</v>
       </c>
       <c r="D5" t="n">
-        <v>1044.69510098896</v>
+        <v>1049.157349251982</v>
       </c>
       <c r="E5" t="n">
-        <v>1042.124039319232</v>
+        <v>1034.3634674952</v>
       </c>
     </row>
     <row r="6">
@@ -1062,16 +1062,16 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1051.42714890711</v>
+        <v>1051.940720376329</v>
       </c>
       <c r="C6" t="n">
-        <v>5.971386287569976</v>
+        <v>6.108840297329175</v>
       </c>
       <c r="D6" t="n">
-        <v>1053.815703422138</v>
+        <v>1054.384256495261</v>
       </c>
       <c r="E6" t="n">
-        <v>1049.038594392082</v>
+        <v>1049.497184257397</v>
       </c>
     </row>
     <row r="7">
@@ -1081,16 +1081,16 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1133.906105685227</v>
+        <v>1129.173830184684</v>
       </c>
       <c r="C7" t="n">
-        <v>25.79761788276344</v>
+        <v>15.63764467499404</v>
       </c>
       <c r="D7" t="n">
-        <v>1144.225152838332</v>
+        <v>1135.428888054682</v>
       </c>
       <c r="E7" t="n">
-        <v>1123.587058532121</v>
+        <v>1122.918772314687</v>
       </c>
     </row>
     <row r="8">
@@ -1100,16 +1100,16 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1150.31791847427</v>
+        <v>1155.315369926075</v>
       </c>
       <c r="C8" t="n">
-        <v>19.86266090914843</v>
+        <v>22.70745094780504</v>
       </c>
       <c r="D8" t="n">
-        <v>1158.262982837929</v>
+        <v>1164.398350305197</v>
       </c>
       <c r="E8" t="n">
-        <v>1142.372854110611</v>
+        <v>1146.232389546953</v>
       </c>
     </row>
     <row r="9">
@@ -1119,16 +1119,16 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>1282.068937550689</v>
+        <v>1261.148905109489</v>
       </c>
       <c r="C9" t="n">
-        <v>32.7124123346662</v>
+        <v>37.56639532440263</v>
       </c>
       <c r="D9" t="n">
-        <v>1295.153902484556</v>
+        <v>1276.17546323925</v>
       </c>
       <c r="E9" t="n">
-        <v>1268.983972616823</v>
+        <v>1246.122346979728</v>
       </c>
     </row>
     <row r="10">
@@ -1138,16 +1138,16 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>1349.018329278183</v>
+        <v>1340.351500405515</v>
       </c>
       <c r="C10" t="n">
-        <v>26.2154802179095</v>
+        <v>54.77242273365485</v>
       </c>
       <c r="D10" t="n">
-        <v>1359.504521365347</v>
+        <v>1362.260469498977</v>
       </c>
       <c r="E10" t="n">
-        <v>1338.53213719102</v>
+        <v>1318.442531312053</v>
       </c>
     </row>
     <row r="11">
@@ -1157,16 +1157,16 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>1400.841362530414</v>
+        <v>1417.669586374696</v>
       </c>
       <c r="C11" t="n">
-        <v>40.37058682613002</v>
+        <v>61.49648747407302</v>
       </c>
       <c r="D11" t="n">
-        <v>1416.989597260866</v>
+        <v>1442.268181364325</v>
       </c>
       <c r="E11" t="n">
-        <v>1384.693127799962</v>
+        <v>1393.070991385067</v>
       </c>
     </row>
     <row r="12">
@@ -1176,16 +1176,16 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>1428.619505271695</v>
+        <v>1420.967653419843</v>
       </c>
       <c r="C12" t="n">
-        <v>39.23947281823583</v>
+        <v>28.50336307935525</v>
       </c>
       <c r="D12" t="n">
-        <v>1444.315294398989</v>
+        <v>1432.368998651585</v>
       </c>
       <c r="E12" t="n">
-        <v>1412.923716144401</v>
+        <v>1409.566308188101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>